<commit_message>
updated changes to code and deleted copy1
</commit_message>
<xml_diff>
--- a/data/raw/week_3_project_data.xlsx
+++ b/data/raw/week_3_project_data.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manht\Desktop\_IRONHACK\Module_1\MiniProjects\Week3\W3GroupLab\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD2B599-B735-45EB-91F8-C859E73733D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="11595" yWindow="4305" windowWidth="28290" windowHeight="15885" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Housing Cost Index" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Rental Cost Index" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Mean Income" sheetId="3" r:id="rId6"/>
+    <sheet name="Housing Cost Index" sheetId="1" r:id="rId1"/>
+    <sheet name="Rental Cost Index" sheetId="2" r:id="rId2"/>
+    <sheet name="Mean Income" sheetId="3" r:id="rId3"/>
+    <sheet name="Mean Minimum Wage" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>DE</t>
   </si>
@@ -22,32 +32,79 @@
   </si>
   <si>
     <t>PT</t>
+  </si>
+  <si>
+    <t>1249.84</t>
+  </si>
+  <si>
+    <t>1271.6</t>
+  </si>
+  <si>
+    <t>1305.6</t>
+  </si>
+  <si>
+    <t>1345.55</t>
+  </si>
+  <si>
+    <t>1684.8</t>
+  </si>
+  <si>
+    <t>1232.18</t>
+  </si>
+  <si>
+    <t>1246.93</t>
+  </si>
+  <si>
+    <t>1287.47</t>
+  </si>
+  <si>
+    <t>1359.95</t>
+  </si>
+  <si>
+    <t>600.00</t>
+  </si>
+  <si>
+    <t>635.00</t>
+  </si>
+  <si>
+    <t>665.00</t>
+  </si>
+  <si>
+    <t>705.00</t>
+  </si>
+  <si>
+    <t>760.00</t>
+  </si>
+  <si>
+    <t>1415.23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="&quot;Arial&quot;"/>
     </font>
@@ -57,7 +114,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -67,56 +124,55 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -306,284 +362,383 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7">
       <c r="B1" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="C1" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="D1" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="E1" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="F1" s="1">
-        <v>2023.0</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+        <v>2023</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
-        <v>128.7</v>
-      </c>
-      <c r="C2" s="4">
-        <v>138.7</v>
-      </c>
-      <c r="D2" s="4">
-        <v>154.8</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="B2" s="3">
+        <v>128.69999999999999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>138.69999999999999</v>
+      </c>
+      <c r="D2" s="3">
+        <v>154.80000000000001</v>
+      </c>
+      <c r="E2" s="3">
         <v>162.6</v>
       </c>
-      <c r="F2" s="4">
-        <v>148.8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="F2" s="3">
+        <v>148.80000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>110.86</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>116.62</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>123.98</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>131.82</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>131.26</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>141.88</v>
       </c>
-      <c r="C4" s="4">
-        <v>154.33</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="3">
+        <v>154.33000000000001</v>
+      </c>
+      <c r="D4" s="3">
         <v>168.84</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>190.17</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>205.76</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7">
       <c r="B1" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="C1" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="D1" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="E1" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="F1" s="1">
-        <v>2023.0</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+        <v>2023</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>100.67</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>101.06</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>101.92</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>102.6</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>104.78</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>107.97</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>110.76</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>101.92</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>115.79</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>121.05</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>106.1</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>107.6</v>
       </c>
-      <c r="D4" s="4">
-        <v>109.0</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="D4" s="3">
+        <v>109</v>
+      </c>
+      <c r="E4" s="3">
         <v>110.8</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>113.1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7">
       <c r="B1" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="C1" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="D1" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="E1" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="F1" s="1">
-        <v>2023.0</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+        <v>2023</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6">
-        <v>26105.0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>29896.0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>29106.0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>28569.0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>30308.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="5">
+        <v>26105</v>
+      </c>
+      <c r="C2" s="5">
+        <v>29896</v>
+      </c>
+      <c r="D2" s="5">
+        <v>29106</v>
+      </c>
+      <c r="E2" s="5">
+        <v>28569</v>
+      </c>
+      <c r="F2" s="5">
+        <v>30308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
-        <v>26210.0</v>
-      </c>
-      <c r="C3" s="7">
-        <v>25382.0</v>
-      </c>
-      <c r="D3" s="7">
-        <v>26075.0</v>
-      </c>
-      <c r="E3" s="7">
-        <v>26419.0</v>
-      </c>
-      <c r="F3" s="7">
-        <v>27577.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="6">
+        <v>26210</v>
+      </c>
+      <c r="C3" s="6">
+        <v>25382</v>
+      </c>
+      <c r="D3" s="6">
+        <v>26075</v>
+      </c>
+      <c r="E3" s="6">
+        <v>26419</v>
+      </c>
+      <c r="F3" s="6">
+        <v>27577</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
-        <v>11786.0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>12696.0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>13113.0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>13148.0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>14368.0</v>
+      <c r="B4" s="5">
+        <v>11786</v>
+      </c>
+      <c r="C4" s="5">
+        <v>12696</v>
+      </c>
+      <c r="D4" s="5">
+        <v>13113</v>
+      </c>
+      <c r="E4" s="5">
+        <v>13148</v>
+      </c>
+      <c r="F4" s="5">
+        <v>14368</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17737B78-C6FD-44FA-BD93-F938805D4ABD}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>